<commit_message>
Completed Birth data creation
</commit_message>
<xml_diff>
--- a/BirthChart.xlsx
+++ b/BirthChart.xlsx
@@ -61,67 +61,64 @@
     <t>SU</t>
   </si>
   <si>
-    <t>Tau</t>
+    <t>Vir</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Good Friend</t>
   </si>
   <si>
     <t>VE</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Neutral</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>MO</t>
-  </si>
-  <si>
-    <t>Friend</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>Ari</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Sco</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>JU</t>
+  </si>
+  <si>
+    <t>Aqu</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>RA</t>
   </si>
   <si>
     <t>Pis</t>
   </si>
   <si>
-    <t>JU</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Cap</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Sco</t>
-  </si>
-  <si>
-    <t>Great Enemy</t>
-  </si>
-  <si>
-    <t>RA</t>
+    <t>8</t>
   </si>
   <si>
     <t>Aries</t>
@@ -160,13 +157,16 @@
     <t>Pisces</t>
   </si>
   <si>
-    <t>ME/RA</t>
-  </si>
-  <si>
-    <t>SU/MO/MA</t>
+    <t>SU/MO/ME/VE/SA</t>
   </si>
   <si>
     <t>Houses</t>
+  </si>
+  <si>
+    <t>ME/VE/SA</t>
+  </si>
+  <si>
+    <t>SU/MO</t>
   </si>
 </sst>
 </file>
@@ -592,28 +592,24 @@
       <c r="E2" s="6" t="n"/>
       <c r="F2" s="6" t="n"/>
       <c r="G2" s="6" t="n"/>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="H2" s="6" t="n"/>
       <c r="I2" s="6" t="n"/>
       <c r="J2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="6" t="n"/>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="6" t="n"/>
+      <c r="M2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="O2" s="6" t="n"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>15</v>
@@ -621,60 +617,56 @@
       <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="D3" s="6" t="n"/>
       <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="6" t="n"/>
+      <c r="F3" s="6" t="n"/>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="H3" s="6" t="n"/>
-      <c r="I3" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="I3" s="6" t="n"/>
       <c r="J3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="6" t="n"/>
       <c r="L3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="O3" s="6" t="n"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="6" t="n"/>
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" s="6" t="n"/>
-      <c r="F4" s="6" t="n"/>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="6" t="n"/>
       <c r="H4" s="6" t="n"/>
-      <c r="I4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="6" t="n"/>
-      <c r="L4" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="I4" s="6" t="n"/>
+      <c r="J4" s="6" t="n"/>
+      <c r="K4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="6" t="n"/>
       <c r="M4" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>19</v>
@@ -683,134 +675,128 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="6" t="n"/>
+      <c r="D5" s="6" t="n"/>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
+      <c r="G5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="H5" s="6" t="n"/>
-      <c r="I5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="6" t="n"/>
+      <c r="I5" s="6" t="n"/>
+      <c r="J5" s="6" t="n"/>
+      <c r="K5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="L5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="O5" s="6" t="n"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="n"/>
       <c r="E6" s="6" t="n"/>
       <c r="F6" s="6" t="n"/>
       <c r="G6" s="6" t="n"/>
       <c r="H6" s="6" t="n"/>
-      <c r="I6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="6" t="n"/>
-      <c r="L6" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="I6" s="6" t="n"/>
+      <c r="J6" s="6" t="n"/>
+      <c r="K6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="6" t="n"/>
       <c r="M6" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O6" s="6" t="n"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="n"/>
-      <c r="E7" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="E7" s="6" t="n"/>
       <c r="F7" s="6" t="n"/>
       <c r="G7" s="6" t="n"/>
       <c r="H7" s="6" t="n"/>
       <c r="I7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="6" t="n"/>
+      <c r="J7" s="6" t="n"/>
+      <c r="K7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="L7" s="6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="O7" s="6" t="n"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D8" s="6" t="n"/>
       <c r="E8" s="6" t="n"/>
       <c r="F8" s="6" t="n"/>
-      <c r="G8" s="6" t="n"/>
-      <c r="H8" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="6" t="n"/>
       <c r="I8" s="6" t="n"/>
       <c r="J8" s="6" t="n"/>
       <c r="K8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>19</v>
@@ -819,34 +805,34 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="6" t="n"/>
       <c r="E9" s="6" t="n"/>
       <c r="F9" s="6" t="n"/>
-      <c r="G9" s="6" t="n"/>
-      <c r="H9" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="6" t="n"/>
       <c r="I9" s="6" t="n"/>
       <c r="J9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="6" t="n"/>
       <c r="L9" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="O9" s="6" t="n"/>
     </row>
@@ -858,62 +844,59 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:15">
+      <c r="G16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
       <c r="I16" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
       </c>
       <c r="M16" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row customFormat="1" r="25" s="4" spans="1:15">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>1</v>
@@ -953,20 +936,20 @@
       </c>
     </row>
     <row r="26" spans="1:15">
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" t="s">
-        <v>48</v>
-      </c>
-      <c r="L26" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="I26" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>